<commit_message>
Appended sheet title to the translation list
</commit_message>
<xml_diff>
--- a/raw_data/translated_chinese_english_dictionary.xlsx
+++ b/raw_data/translated_chinese_english_dictionary.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C808"/>
+  <dimension ref="A1:C827"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12474,6 +12474,291 @@
         </is>
       </c>
     </row>
+    <row r="809">
+      <c r="A809">
+        <v>808</v>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>食材单价</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>Ingredients price</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810">
+        <v>809</v>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>海南雞飯</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>Hainan Chicken</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811">
+        <v>810</v>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>肉骨茶</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>Bak Kut Tea</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812">
+        <v>811</v>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>海南雞叻沙套餐</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>Hainan Chicken Laksa Set</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813">
+        <v>812</v>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>海南鸡肉骨茶套餐</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>Hainan Chicken Kow Teh Set Meal</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814">
+        <v>813</v>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>龙虾叻沙</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>Lobster Laksa</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815">
+        <v>814</v>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>肥牛叻沙</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>Fatty Niu Laksa</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816">
+        <v>815</v>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>大虾叻沙</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>Big shrimp laksa</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817">
+        <v>816</v>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>海南雞叻沙</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>Hainan Chi Laksa</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818">
+        <v>817</v>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>米暹</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>Mi Siam</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819">
+        <v>818</v>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>咖哩雞</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>Curry Chicken</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820">
+        <v>819</v>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>海南椰子鸡汤米</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>Hainan Coconut Chicken Soup</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821">
+        <v>820</v>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>鸡丝面</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>Chicken Shred Noodle</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822">
+        <v>821</v>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>虾面汤</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>Shrimp Noodle Soup</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823">
+        <v>822</v>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>马拉卤面</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>Mara balsamic noodle</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824">
+        <v>823</v>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>自家制叻沙酱</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>Homemade laksa sauce</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825">
+        <v>824</v>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>新加坡酱汁茶粉报价</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>Singapore sauce tea powder quote</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826">
+        <v>825</v>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>咖椰糯米饭</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>Kaya glutinous rice</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827">
+        <v>826</v>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>娘惹炸鸡翼</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>Nyonya Fried Chicken Wings</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>